<commit_message>
intial commit for flask environment
</commit_message>
<xml_diff>
--- a/dbschema.xlsx
+++ b/dbschema.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\_PYTHON\NocLightScottsdale\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\_PYTHON\noc-light-scottsdale\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13905" windowHeight="7590" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13905" windowHeight="7590" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="noclightaz" sheetId="1" r:id="rId1"/>
@@ -26,20 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
-  <si>
-    <t>ContentViewers/EdgeStatus/FullStatus</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>minRealm</t>
-  </si>
-  <si>
-    <t>maxRealm</t>
-  </si>
-  <si>
     <t>core.learn.edgenuity.com</t>
   </si>
   <si>
@@ -64,36 +55,9 @@
     <t>type</t>
   </si>
   <si>
-    <t>QuestionAPI/api/EdgeStatus/FullStatus</t>
-  </si>
-  <si>
-    <t>ContentEngineAPI/api/EdgeStatus/FullStatus</t>
-  </si>
-  <si>
-    <t>student/EdgeStatus/FullStatus</t>
-  </si>
-  <si>
-    <t>Educator/EdgeStatus/FullStatus</t>
-  </si>
-  <si>
-    <t>Family/EdgeStatus/FullStatus</t>
-  </si>
-  <si>
-    <t>LMSAPI/req/EdgeStatus/FullStatus</t>
-  </si>
-  <si>
-    <t>Player/EdgeStatus/FullStatus</t>
-  </si>
-  <si>
     <t>http://a{x}</t>
   </si>
   <si>
-    <t>:9624/api/status</t>
-  </si>
-  <si>
-    <t>port</t>
-  </si>
-  <si>
     <t>/ContentViewers/EdgeStatus/FullStatus</t>
   </si>
   <si>
@@ -149,6 +113,39 @@
   </si>
   <si>
     <t>http://a{x}-rpl-tsk01-x:{y}/api/status</t>
+  </si>
+  <si>
+    <t>urlEndpoint</t>
+  </si>
+  <si>
+    <t>https://learn.education2020.com/educator/monitor.aspx</t>
+  </si>
+  <si>
+    <t>https://learn.education2020.com/contentviewers/monitor</t>
+  </si>
+  <si>
+    <t>http://auth.edgenuity.com/login/login/student</t>
+  </si>
+  <si>
+    <t>http://auth.edgenuity.com/login/login/educator</t>
+  </si>
+  <si>
+    <t>https://edgenuity.slack.com</t>
+  </si>
+  <si>
+    <t>http://core.learn.edgenuity.com/platformsynthesizer/EdgeStatus/FullStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://cp.edgenuity.com/Contentplatform/api/EdgeStatus/FullStatus </t>
+  </si>
+  <si>
+    <t>http://auth.edgenuity.com/Login/EdgeStatus/FullStatus</t>
+  </si>
+  <si>
+    <t>http://auth.edgenuity.com/AuthenticationAPI/req/EdgeStatus/FullStatus</t>
+  </si>
+  <si>
+    <t>http://tools.core.learn.edgenuity.com/businessapi/api/EdgeStatus/FullStatus</t>
   </si>
 </sst>
 </file>
@@ -512,13 +509,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="str">
@@ -533,17 +530,17 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="str">
-        <f t="shared" ref="E3:E10" si="0">CONCATENATE(A3,B3,C3)</f>
+        <f t="shared" ref="E3:E9" si="0">CONCATENATE(A3,B3,C3)</f>
         <v>http://r{x}.core.learn.edgenuity.com/QuestionAPI/api/EdgeStatus/FullStatus</v>
       </c>
       <c r="F3" s="2"/>
@@ -554,13 +551,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="str">
@@ -575,13 +572,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="str">
@@ -596,13 +593,13 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="str">
@@ -617,13 +614,13 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="str">
@@ -638,13 +635,13 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="str">
@@ -659,13 +656,13 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="str">
@@ -695,7 +692,7 @@
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="E11" s="5" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -709,7 +706,7 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -723,7 +720,7 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -737,7 +734,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -751,7 +748,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="4"/>
       <c r="E15" s="2" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -765,7 +762,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -779,7 +776,7 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -793,7 +790,7 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1027,122 +1024,120 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G11"/>
+  <dimension ref="B1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="41.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="11" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="72" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="1">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="1">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="1">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="1">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="1">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="1">
-        <v>5</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="1">
-        <v>5</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="1">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>20</v>
+      <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C11" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1150,7 +1145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -1164,24 +1159,24 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -1189,10 +1184,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -1200,7 +1195,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -1209,7 +1204,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -1218,7 +1213,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -1227,7 +1222,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1236,7 +1231,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -1245,7 +1240,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D9">
         <v>5</v>
@@ -1260,7 +1255,7 @@
         <v>9624</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1268,7 +1263,7 @@
         <v>9000</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>